<commit_message>
few updates on SHACL and XSL
</commit_message>
<xml_diff>
--- a/05-Dataset5_org-ap-ep/04-SHACL/Dataset5_MEP-Shapes.xlsx
+++ b/05-Dataset5_org-ap-ep/04-SHACL/Dataset5_MEP-Shapes.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="class-based shapes" sheetId="1" state="visible" r:id="rId2"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="449" uniqueCount="233">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="450" uniqueCount="234">
   <si>
     <t xml:space="preserve">Shapes URI</t>
   </si>
@@ -220,492 +220,6 @@
   </si>
   <si>
     <t xml:space="preserve">Contact Point info for a MEP</t>
-  </si>
-  <si>
-    <t xml:space="preserve">"^http://data.europarl.europa.eu/resource/contact-point/electronic/[0-9]{1,6}/.*$"</t>
-  </si>
-  <si>
-    <t xml:space="preserve">References to external classes</t>
-  </si>
-  <si>
-    <t xml:space="preserve">epsh:Country</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Pays</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Country</t>
-  </si>
-  <si>
-    <t xml:space="preserve">"^http://publications.europa.eu/resource/authority/country/.*$"</t>
-  </si>
-  <si>
-    <t xml:space="preserve">epsh:Place</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Lieu</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Place</t>
-  </si>
-  <si>
-    <t xml:space="preserve">"^http://publications.europa.eu/resource/authority/place/.*$"</t>
-  </si>
-  <si>
-    <t xml:space="preserve">epsh:Civility</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Civilité</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Civility</t>
-  </si>
-  <si>
-    <t xml:space="preserve">"^http://data.europarl.europa.eu/authority/civility/.*$"</t>
-  </si>
-  <si>
-    <t xml:space="preserve">epsh:ContactPointType</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Type d’information de contact</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Contact Point Type</t>
-  </si>
-  <si>
-    <t xml:space="preserve">"^http://data.europarl.europa.eu/authority/contact-point-type/.*$"</t>
-  </si>
-  <si>
-    <t xml:space="preserve">epsh:Gender</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Genre</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Gender</t>
-  </si>
-  <si>
-    <t xml:space="preserve">"^http://data.europarl.europa.eu/authority/gender/.*$"</t>
-  </si>
-  <si>
-    <t xml:space="preserve">epsh:ParliamentaryTerm</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Législature</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Parliamentary Term</t>
-  </si>
-  <si>
-    <t xml:space="preserve">"^http://data.europarl.europa.eu/authority/parliamentary-term/[0-9][0-9]?$"</t>
-  </si>
-  <si>
-    <t xml:space="preserve">epsh:MembershipType</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Type d’appartenance</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Membership Type</t>
-  </si>
-  <si>
-    <t xml:space="preserve">"^http://data.europarl.europa.eu/authority/membership-type/.*$"</t>
-  </si>
-  <si>
-    <t xml:space="preserve">epsh:Function</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Fonction</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Function</t>
-  </si>
-  <si>
-    <t xml:space="preserve">"^http://data.europarl.europa.eu/authority/function/.*$"</t>
-  </si>
-  <si>
-    <t xml:space="preserve">epsh:Constituency</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Constituency</t>
-  </si>
-  <si>
-    <t xml:space="preserve">"^http://data.europarl.europa.eu/authority/constituency/.*-.*$"</t>
-  </si>
-  <si>
-    <t xml:space="preserve">epsh:Organization</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Organisation</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Organization</t>
-  </si>
-  <si>
-    <t xml:space="preserve">"^http://data.europarl.europa.eu/org/.*-.*$"</t>
-  </si>
-  <si>
-    <t xml:space="preserve">epsh:Site</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Site</t>
-  </si>
-  <si>
-    <t xml:space="preserve">"^http://publications.europa.eu/resource/authority/site/.*$"</t>
-  </si>
-  <si>
-    <t xml:space="preserve">This sheet specifies constraints that are attached to the NodeShapes specified in the first sheet</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Constraint IRI</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Predicate or path on which the constraint applies</t>
-  </si>
-  <si>
-    <t xml:space="preserve">NodeShape to which the constraint is applied (a reference to a NodeShape IRI from the first sheet)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Display order of the property / constraint</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Name of predicate/path within the context of that NodeShape</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Description of the predicate/path within the context of that NodeShape</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Type of nodes that the values must have (sh:IRI or sh:Literal)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Minimum cardinality that the predicate/path must have</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Maximum cardinality that the predicate/path must have</t>
-  </si>
-  <si>
-    <t xml:space="preserve">For literal values, the expected datatype of the values</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Expected class that the values of the predicate/path must have, if only one</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Expected shape that the values of the predicate/path must follow.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">General URI or string pattern expected for the values of the predicate/path, expressed as a regex</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Expected classes that the values of the predicate/path must have, if there are multiple. Expressed as a Turtle list.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The shape that must be verified by the qualifiedMin or qualifiedMax count</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Minimum number of time that the shape indicated by sh:qualifiedValueShape must be found</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Maximum number of times that the shape indicated by sh:qualifiedValueShape must be found</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Expected possible values for the predicate/path, when the list is small and known in advance. Expressed as a Turtle list</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Set to true for skos:prefLabel to indicate there should be only one value per langage</t>
-  </si>
-  <si>
-    <t xml:space="preserve">List of langage codes expected for this predicate/path. Expressed as a turtle list</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Allowed value, when there is only one</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sh:path</t>
-  </si>
-  <si>
-    <t xml:space="preserve">^sh:property(separator=",")</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sh:name@en</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sh:description</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sh:minCount^^xsd:integer</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sh:maxCount^^xsd:integer</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sh:datatype</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sh:class</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sh:node</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sh:or</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sh:qualifiedValueShape</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sh:qualifiedMinCount^^xsd:integer</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sh:qualifiedMaxCount^^xsd:integer</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sh:in</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sh:uniqueLang^^xsd:boolean</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sh:languageIn</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sh:hasValue</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Constraints on MEP</t>
-  </si>
-  <si>
-    <t xml:space="preserve">foaf:firstName</t>
-  </si>
-  <si>
-    <t xml:space="preserve">first name</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sh:Literal</t>
-  </si>
-  <si>
-    <t xml:space="preserve">xsd:string</t>
-  </si>
-  <si>
-    <t xml:space="preserve">foaf:familyName</t>
-  </si>
-  <si>
-    <t xml:space="preserve">family name</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ep-org:upperFirstName</t>
-  </si>
-  <si>
-    <t xml:space="preserve">upper first name</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ep-org:upperFamilyName</t>
-  </si>
-  <si>
-    <t xml:space="preserve">upper family name</t>
-  </si>
-  <si>
-    <t xml:space="preserve">schema:honorificPrefix</t>
-  </si>
-  <si>
-    <t xml:space="preserve">civility</t>
-  </si>
-  <si>
-    <t xml:space="preserve">schema:gender</t>
-  </si>
-  <si>
-    <t xml:space="preserve">gender</t>
-  </si>
-  <si>
-    <t xml:space="preserve">schema:birthPlace</t>
-  </si>
-  <si>
-    <t xml:space="preserve">birth place</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ep-org:curriculumVitae</t>
-  </si>
-  <si>
-    <t xml:space="preserve">curriculum vitae</t>
-  </si>
-  <si>
-    <t xml:space="preserve">rdf:langString</t>
-  </si>
-  <si>
-    <t xml:space="preserve">("fr" "en")</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ep-org:dateEndActivity</t>
-  </si>
-  <si>
-    <t xml:space="preserve">date end of activity</t>
-  </si>
-  <si>
-    <t xml:space="preserve">xsd:dateTime</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ep-org:personId</t>
-  </si>
-  <si>
-    <t xml:space="preserve">person ID</t>
-  </si>
-  <si>
-    <t xml:space="preserve">schema:birthDate</t>
-  </si>
-  <si>
-    <t xml:space="preserve">birth date</t>
-  </si>
-  <si>
-    <t xml:space="preserve">foaf:img</t>
-  </si>
-  <si>
-    <t xml:space="preserve">image</t>
-  </si>
-  <si>
-    <t xml:space="preserve">schema:nationality</t>
-  </si>
-  <si>
-    <t xml:space="preserve">nationality</t>
-  </si>
-  <si>
-    <t xml:space="preserve">schema:contactPoint</t>
-  </si>
-  <si>
-    <t xml:space="preserve">contact point</t>
-  </si>
-  <si>
-    <t xml:space="preserve">org:hasMembership</t>
-  </si>
-  <si>
-    <t xml:space="preserve">membership</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Constraints on ContactPoint</t>
-  </si>
-  <si>
-    <t xml:space="preserve">schema:contactType</t>
-  </si>
-  <si>
-    <t xml:space="preserve">contact type</t>
-  </si>
-  <si>
-    <t xml:space="preserve">schema:url</t>
-  </si>
-  <si>
-    <t xml:space="preserve">url</t>
-  </si>
-  <si>
-    <t xml:space="preserve">schema:telephone</t>
-  </si>
-  <si>
-    <t xml:space="preserve">telephone</t>
-  </si>
-  <si>
-    <t xml:space="preserve">schema:faxNumber</t>
-  </si>
-  <si>
-    <t xml:space="preserve">fax number</t>
-  </si>
-  <si>
-    <t xml:space="preserve">schema:email</t>
-  </si>
-  <si>
-    <t xml:space="preserve">email</t>
-  </si>
-  <si>
-    <t xml:space="preserve">schema:addressCountry</t>
-  </si>
-  <si>
-    <t xml:space="preserve">address country</t>
-  </si>
-  <si>
-    <t xml:space="preserve">schema:addressLocality</t>
-  </si>
-  <si>
-    <t xml:space="preserve">address locality</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ep-org:hasSite</t>
-  </si>
-  <si>
-    <t xml:space="preserve">has site</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ep-org:officeId</t>
-  </si>
-  <si>
-    <t xml:space="preserve">office ID</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Constraints on Membership MEP</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ep-org:hasMembershipType</t>
-  </si>
-  <si>
-    <t xml:space="preserve">membership type</t>
-  </si>
-  <si>
-    <t xml:space="preserve">schema:startDate</t>
-  </si>
-  <si>
-    <t xml:space="preserve">start date</t>
-  </si>
-  <si>
-    <t xml:space="preserve">schema:endDate</t>
-  </si>
-  <si>
-    <t xml:space="preserve">end date</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ep-org:hasOrganization</t>
-  </si>
-  <si>
-    <t xml:space="preserve">country</t>
-  </si>
-  <si>
-    <t xml:space="preserve">([sh:node epsh:Organization] [sh:node epsh:Country])</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ep-org:hasParliamentaryTerm</t>
-  </si>
-  <si>
-    <t xml:space="preserve">parliamentary term</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ep-org:constituency</t>
-  </si>
-  <si>
-    <t xml:space="preserve">constituency</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ep-org:hasMembershipBasedOn</t>
-  </si>
-  <si>
-    <t xml:space="preserve">based on</t>
-  </si>
-  <si>
-    <t xml:space="preserve">org:role</t>
-  </si>
-  <si>
-    <t xml:space="preserve">role</t>
-  </si>
-  <si>
-    <t xml:space="preserve">epsh:Role</t>
-  </si>
-  <si>
-    <t xml:space="preserve">dc:identifier</t>
-  </si>
-  <si>
-    <t xml:space="preserve">mandate id (only on mandates)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Constraints on Assistants</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ep-org:hasPersonType</t>
-  </si>
-  <si>
-    <t xml:space="preserve">person type</t>
   </si>
   <si>
     <r>
@@ -715,7 +229,7 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">( &lt;</t>
+      <t xml:space="preserve">"^</t>
     </r>
     <r>
       <rPr>
@@ -725,7 +239,7 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">http://data.europarl.europa.eu/authority/person-type/AST-APA</t>
+      <t xml:space="preserve">http://data.europarl.europa.eu/resource/contact-point/(electronic</t>
     </r>
     <r>
       <rPr>
@@ -734,46 +248,497 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">&gt; &lt;</t>
+      <t xml:space="preserve">|place)/[0-9]{1,6}/.*$"</t>
     </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF0000FF"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">http://data.europarl.europa.eu/authority/person-type/AST-APA-GRP</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">&gt; &lt;</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF0000FF"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">http://data.europarl.europa.eu/authority/person-type/AST-LOC</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">&gt; )</t>
-    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">References to external classes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">epsh:Country</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pays</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Country</t>
+  </si>
+  <si>
+    <t xml:space="preserve">"^http://publications.europa.eu/resource/authority/country/.*$"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">epsh:Place</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lieu</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Place</t>
+  </si>
+  <si>
+    <t xml:space="preserve">"^http://publications.europa.eu/resource/authority/place/.*$"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">epsh:Civility</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Civilité</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Civility</t>
+  </si>
+  <si>
+    <t xml:space="preserve">"^http://data.europarl.europa.eu/authority/civility/.*$"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">epsh:ContactPointType</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Type d’information de contact</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Contact Point Type</t>
+  </si>
+  <si>
+    <t xml:space="preserve">"^http://data.europarl.europa.eu/authority/contact-point-type/.*$"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">epsh:Gender</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Genre</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gender</t>
+  </si>
+  <si>
+    <t xml:space="preserve">"^http://data.europarl.europa.eu/authority/gender/.*$"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">epsh:ParliamentaryTerm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Législature</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Parliamentary Term</t>
+  </si>
+  <si>
+    <t xml:space="preserve">"^http://data.europarl.europa.eu/authority/parliamentary-term/[0-9][0-9]?$"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">epsh:MembershipType</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Type d’appartenance</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Membership Type</t>
+  </si>
+  <si>
+    <t xml:space="preserve">"^http://data.europarl.europa.eu/authority/membership-type/.*$"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">epsh:Function</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fonction</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Function</t>
+  </si>
+  <si>
+    <t xml:space="preserve">"^http://data.europarl.europa.eu/authority/function/.*$"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">epsh:Constituency</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Constituency</t>
+  </si>
+  <si>
+    <t xml:space="preserve">"^http://data.europarl.europa.eu/authority/constituency/.*-.*$"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">epsh:Organization</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Organisation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Organization</t>
+  </si>
+  <si>
+    <t xml:space="preserve">"^http://data.europarl.europa.eu/org/.*-.*$"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">epsh:Site</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Site</t>
+  </si>
+  <si>
+    <t xml:space="preserve">"^http://publications.europa.eu/resource/authority/site/.*$"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">This sheet specifies constraints that are attached to the NodeShapes specified in the first sheet</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Constraint IRI</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Predicate or path on which the constraint applies</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NodeShape to which the constraint is applied (a reference to a NodeShape IRI from the first sheet)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Display order of the property / constraint</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Name of predicate/path within the context of that NodeShape</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Description of the predicate/path within the context of that NodeShape</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Type of nodes that the values must have (sh:IRI or sh:Literal)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Minimum cardinality that the predicate/path must have</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Maximum cardinality that the predicate/path must have</t>
+  </si>
+  <si>
+    <t xml:space="preserve">For literal values, the expected datatype of the values</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Expected class that the values of the predicate/path must have, if only one</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Expected shape that the values of the predicate/path must follow.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">General URI or string pattern expected for the values of the predicate/path, expressed as a regex</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Expected classes that the values of the predicate/path must have, if there are multiple. Expressed as a Turtle list.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The shape that must be verified by the qualifiedMin or qualifiedMax count</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Minimum number of time that the shape indicated by sh:qualifiedValueShape must be found</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Maximum number of times that the shape indicated by sh:qualifiedValueShape must be found</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Expected possible values for the predicate/path, when the list is small and known in advance. Expressed as a Turtle list</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Set to true for skos:prefLabel to indicate there should be only one value per langage</t>
+  </si>
+  <si>
+    <t xml:space="preserve">List of langage codes expected for this predicate/path. Expressed as a turtle list</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Allowed value, when there is only one</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sh:path</t>
+  </si>
+  <si>
+    <t xml:space="preserve">^sh:property(separator=",")</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sh:name@en</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sh:description</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sh:minCount^^xsd:integer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sh:maxCount^^xsd:integer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sh:datatype</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sh:class</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sh:node</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sh:or</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sh:qualifiedValueShape</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sh:qualifiedMinCount^^xsd:integer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sh:qualifiedMaxCount^^xsd:integer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sh:in</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sh:uniqueLang^^xsd:boolean</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sh:languageIn</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sh:hasValue</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Constraints on MEP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">foaf:firstName</t>
+  </si>
+  <si>
+    <t xml:space="preserve">first name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sh:Literal</t>
+  </si>
+  <si>
+    <t xml:space="preserve">xsd:string</t>
+  </si>
+  <si>
+    <t xml:space="preserve">foaf:familyName</t>
+  </si>
+  <si>
+    <t xml:space="preserve">family name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ep-org:upperFirstName</t>
+  </si>
+  <si>
+    <t xml:space="preserve">upper first name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ep-org:upperFamilyName</t>
+  </si>
+  <si>
+    <t xml:space="preserve">upper family name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">schema:honorificPrefix</t>
+  </si>
+  <si>
+    <t xml:space="preserve">civility</t>
+  </si>
+  <si>
+    <t xml:space="preserve">schema:gender</t>
+  </si>
+  <si>
+    <t xml:space="preserve">gender</t>
+  </si>
+  <si>
+    <t xml:space="preserve">schema:birthPlace</t>
+  </si>
+  <si>
+    <t xml:space="preserve">birth place</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ep-org:curriculumVitae</t>
+  </si>
+  <si>
+    <t xml:space="preserve">curriculum vitae</t>
+  </si>
+  <si>
+    <t xml:space="preserve">rdf:langString</t>
+  </si>
+  <si>
+    <t xml:space="preserve">("fr" "en")</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ep-org:dateEndActivity</t>
+  </si>
+  <si>
+    <t xml:space="preserve">date end of activity</t>
+  </si>
+  <si>
+    <t xml:space="preserve">xsd:dateTime</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ep-org:personId</t>
+  </si>
+  <si>
+    <t xml:space="preserve">person ID</t>
+  </si>
+  <si>
+    <t xml:space="preserve">schema:birthDate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">birth date</t>
+  </si>
+  <si>
+    <t xml:space="preserve">foaf:img</t>
+  </si>
+  <si>
+    <t xml:space="preserve">image</t>
+  </si>
+  <si>
+    <t xml:space="preserve">schema:nationality</t>
+  </si>
+  <si>
+    <t xml:space="preserve">nationality</t>
+  </si>
+  <si>
+    <t xml:space="preserve">schema:contactPoint</t>
+  </si>
+  <si>
+    <t xml:space="preserve">contact point</t>
+  </si>
+  <si>
+    <t xml:space="preserve">org:hasMembership</t>
+  </si>
+  <si>
+    <t xml:space="preserve">membership</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Constraints on ContactPoint</t>
+  </si>
+  <si>
+    <t xml:space="preserve">schema:contactType</t>
+  </si>
+  <si>
+    <t xml:space="preserve">contact type</t>
+  </si>
+  <si>
+    <t xml:space="preserve">schema:url</t>
+  </si>
+  <si>
+    <t xml:space="preserve">url</t>
+  </si>
+  <si>
+    <t xml:space="preserve">schema:telephone</t>
+  </si>
+  <si>
+    <t xml:space="preserve">telephone</t>
+  </si>
+  <si>
+    <t xml:space="preserve">schema:faxNumber</t>
+  </si>
+  <si>
+    <t xml:space="preserve">fax number</t>
+  </si>
+  <si>
+    <t xml:space="preserve">schema:email</t>
+  </si>
+  <si>
+    <t xml:space="preserve">email</t>
+  </si>
+  <si>
+    <t xml:space="preserve">schema:addressCountry</t>
+  </si>
+  <si>
+    <t xml:space="preserve">address country</t>
+  </si>
+  <si>
+    <t xml:space="preserve">schema:addressLocality</t>
+  </si>
+  <si>
+    <t xml:space="preserve">address locality</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ep-org:hasSite</t>
+  </si>
+  <si>
+    <t xml:space="preserve">has site</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ep-org:officeId</t>
+  </si>
+  <si>
+    <t xml:space="preserve">office ID</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Constraints on Membership MEP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ep-org:hasMembershipType</t>
+  </si>
+  <si>
+    <t xml:space="preserve">membership type</t>
+  </si>
+  <si>
+    <t xml:space="preserve">schema:startDate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">start date</t>
+  </si>
+  <si>
+    <t xml:space="preserve">schema:endDate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">end date</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ep-org:hasOrganization</t>
+  </si>
+  <si>
+    <t xml:space="preserve">country</t>
+  </si>
+  <si>
+    <t xml:space="preserve">([sh:node epsh:Organization] [sh:node epsh:Country])</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ep-org:hasParliamentaryTerm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">parliamentary term</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ep-org:constituency</t>
+  </si>
+  <si>
+    <t xml:space="preserve">constituency</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ep-org:hasMembershipBasedOn</t>
+  </si>
+  <si>
+    <t xml:space="preserve">based on</t>
+  </si>
+  <si>
+    <t xml:space="preserve">org:role</t>
+  </si>
+  <si>
+    <t xml:space="preserve">role</t>
+  </si>
+  <si>
+    <t xml:space="preserve">We cannot enforce a minimum cardinality because mandates don’t have a based on</t>
+  </si>
+  <si>
+    <t xml:space="preserve">epsh:Role</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dc:identifier</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mandate id (only on mandates)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Constraints on Assistants</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ep-org:hasPersonType</t>
+  </si>
+  <si>
+    <t xml:space="preserve">person type</t>
+  </si>
+  <si>
+    <t xml:space="preserve">( &lt;http://data.europarl.europa.eu/authority/person-type/AST-APA&gt; &lt;http://data.europarl.europa.eu/authority/person-type/AST-APA-GRP&gt; &lt;http://data.europarl.europa.eu/authority/person-type/AST-LOC&gt; )</t>
   </si>
   <si>
     <t xml:space="preserve">has membership</t>
@@ -1138,11 +1103,11 @@
   </sheetPr>
   <dimension ref="A1:M29"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="G1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="K26" activeCellId="0" sqref="K26"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="G1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="K16" activeCellId="0" sqref="K16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.61328125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="39.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="27.58"/>
@@ -1496,7 +1461,7 @@
       <c r="J15" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="K15" s="14" t="s">
+      <c r="K15" s="0" t="s">
         <v>65</v>
       </c>
       <c r="L15" s="1" t="s">
@@ -1857,7 +1822,7 @@
     <hyperlink ref="K11" r:id="rId5" display="&quot;^http://data.europarl.europa.eu/person/[0-9]{1,6}$&quot;"/>
     <hyperlink ref="K13" r:id="rId6" display="&quot;^http://data.europarl.europa.eu/person/[0-9]{1,6}$&quot;"/>
     <hyperlink ref="K14" r:id="rId7" display="&quot;^http://data.europarl.europa.eu/person/[0-9]{1,6}/membership/[0-9]{1,6}$&quot;"/>
-    <hyperlink ref="K15" r:id="rId8" display="&quot;^http://data.europarl.europa.eu/resource/contact-point/electronic/[0-9]{1,6}/.*$&quot;"/>
+    <hyperlink ref="K15" r:id="rId8" display="http://data.europarl.europa.eu/resource/contact-point/(electronic"/>
     <hyperlink ref="K19" r:id="rId9" display="&quot;^http://publications.europa.eu/resource/authority/country/.*$&quot;"/>
     <hyperlink ref="K20" r:id="rId10" display="&quot;^http://publications.europa.eu/resource/authority/place/.*$&quot;"/>
     <hyperlink ref="K21" r:id="rId11" display="&quot;^http://data.europarl.europa.eu/authority/civility/.*$&quot;"/>
@@ -1886,13 +1851,13 @@
   </sheetPr>
   <dimension ref="A1:AMJ61"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="8" topLeftCell="A21" activePane="bottomLeft" state="frozen"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="0" ySplit="8" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="B41" activeCellId="0" sqref="B41"/>
+      <selection pane="bottomLeft" activeCell="H19" activeCellId="0" sqref="H19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7578125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.76953125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="19.31"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="36.99"/>
@@ -2392,7 +2357,7 @@
         <v>151</v>
       </c>
       <c r="H18" s="1" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I18" s="0" t="n">
         <v>1</v>
@@ -3091,7 +3056,7 @@
         <v>42</v>
       </c>
       <c r="H44" s="1" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I44" s="0" t="n">
         <v>1</v>
@@ -3101,7 +3066,7 @@
       </c>
       <c r="M44" s="14"/>
     </row>
-    <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="45" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="0" t="str">
         <f aca="false">CONCATENATE("epsh:P",ROW(A45))</f>
         <v>epsh:P45</v>
@@ -3118,6 +3083,9 @@
       <c r="E45" s="0" t="s">
         <v>220</v>
       </c>
+      <c r="F45" s="1" t="s">
+        <v>221</v>
+      </c>
       <c r="G45" s="0" t="s">
         <v>42</v>
       </c>
@@ -3128,7 +3096,7 @@
         <v>1</v>
       </c>
       <c r="L45" s="0" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="M45" s="14"/>
     </row>
@@ -3138,7 +3106,7 @@
         <v>epsh:P46</v>
       </c>
       <c r="B46" s="0" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="C46" s="1" t="s">
         <v>46</v>
@@ -3147,7 +3115,7 @@
         <v>9</v>
       </c>
       <c r="E46" s="0" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="G46" s="0" t="s">
         <v>151</v>
@@ -3165,7 +3133,7 @@
     </row>
     <row r="48" s="22" customFormat="true" ht="40.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A48" s="22" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="T48" s="23"/>
       <c r="AMJ48" s="0"/>
@@ -3299,7 +3267,7 @@
         <v>epsh:P53</v>
       </c>
       <c r="B53" s="0" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="C53" s="1" t="s">
         <v>50</v>
@@ -3308,7 +3276,7 @@
         <v>5</v>
       </c>
       <c r="E53" s="0" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="G53" s="0" t="s">
         <v>42</v>
@@ -3319,8 +3287,8 @@
       <c r="I53" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="R53" s="0" t="s">
-        <v>227</v>
+      <c r="R53" s="14" t="s">
+        <v>228</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3368,7 +3336,7 @@
         <v>7</v>
       </c>
       <c r="E55" s="0" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="G55" s="0" t="s">
         <v>42</v>
@@ -3385,7 +3353,7 @@
     </row>
     <row r="58" s="22" customFormat="true" ht="40.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A58" s="22" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="T58" s="23"/>
       <c r="AMJ58" s="0"/>
@@ -3418,7 +3386,7 @@
       </c>
       <c r="M59" s="14"/>
       <c r="U59" s="14" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3468,7 +3436,7 @@
         <v>3</v>
       </c>
       <c r="E61" s="0" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="G61" s="0" t="s">
         <v>42</v>
@@ -3481,14 +3449,14 @@
       </c>
       <c r="M61" s="14"/>
       <c r="U61" s="14" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B1" r:id="rId1" display="http://data.europarl.europa.eu/shapes/meps"/>
     <hyperlink ref="E8" r:id="rId2" display="sh:name@en"/>
-    <hyperlink ref="R53" r:id="rId3" display="http://data.europarl.europa.eu/authority/person-type/AST-APA-GRP"/>
+    <hyperlink ref="R53" r:id="rId3" display="( &lt;http://data.europarl.europa.eu/authority/person-type/AST-APA&gt; &lt;http://data.europarl.europa.eu/authority/person-type/AST-APA-GRP&gt; &lt;http://data.europarl.europa.eu/authority/person-type/AST-LOC&gt; )"/>
     <hyperlink ref="U59" r:id="rId4" display="http://data.europarl.europa.eu/authority/membership-type/PERSON"/>
     <hyperlink ref="U61" r:id="rId5" display="http://data.europarl.europa.eu/authority/function/ASSISTANT"/>
   </hyperlinks>

</xml_diff>